<commit_message>
added code snippet for raw files in R
</commit_message>
<xml_diff>
--- a/_site/content/code-snippets.xlsx
+++ b/_site/content/code-snippets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raincorporate-my.sharepoint.com/personal/vebashini_rain_co_za/Documents/Documents/Main-Documents/Personal/Blog_Vebash/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{ACFAD094-D8EA-4FAF-B074-F0F2496E58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61D5AE69-EB34-4147-AA2D-E498362ADC08}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{ACFAD094-D8EA-4FAF-B074-F0F2496E58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3DCBDE-E7F1-4586-AFA9-4230A0C76E58}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-2200" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>title</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>R; Read Password Protected Excel</t>
+  </si>
+  <si>
+    <t>Raw Strings in R</t>
+  </si>
+  <si>
+    <t>https://sciencificity.github.io/raw-strings-r/</t>
+  </si>
+  <si>
+    <t>R; Raw Strings in R</t>
+  </si>
+  <si>
+    <t>images/mae-mu--dyxcGiP-rE-unsplash1.jpg</t>
+  </si>
+  <si>
+    <t>In Version 4.0.0 of R raw strings were added r"(...)"</t>
   </si>
 </sst>
 </file>
@@ -401,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,11 +499,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EFCDE127-97E1-4BE0-94AA-C496E3B749CF}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{40BE7616-A0C8-414F-A387-6E215007A00D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a code snippet to convert R file to Rmd
</commit_message>
<xml_diff>
--- a/_site/content/code-snippets.xlsx
+++ b/_site/content/code-snippets.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raincorporate-my.sharepoint.com/personal/vebashini_rain_co_za/Documents/Documents/Main-Documents/Personal/Blog_Vebash/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{ACFAD094-D8EA-4FAF-B074-F0F2496E58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3DCBDE-E7F1-4586-AFA9-4230A0C76E58}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{ACFAD094-D8EA-4FAF-B074-F0F2496E58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{340CFB8B-72FE-4AAE-92D3-CBFBE05A65A8}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-2200" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>title</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>In Version 4.0.0 of R raw strings were added r"(...)"</t>
+  </si>
+  <si>
+    <t>Convert an `R` file into an Rmd</t>
+  </si>
+  <si>
+    <t>Use knitr::spin() to convert R file into Rmd</t>
+  </si>
+  <si>
+    <t>R; Convert to Rmd</t>
+  </si>
+  <si>
+    <t>https://github.com/sciencificity/convert-r-to-rmd</t>
+  </si>
+  <si>
+    <t>images/markus-spiske-hGb5WqRrWIg-unsplash.jpg</t>
   </si>
 </sst>
 </file>
@@ -416,18 +431,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -522,12 +538,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EFCDE127-97E1-4BE0-94AA-C496E3B749CF}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{40BE7616-A0C8-414F-A387-6E215007A00D}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{921C780A-61CE-4A77-B664-9B2D9B6D7079}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a snippet for rendering Rmd without plots or results by using code chunk options
</commit_message>
<xml_diff>
--- a/_site/content/code-snippets.xlsx
+++ b/_site/content/code-snippets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raincorporate-my.sharepoint.com/personal/vebashini_rain_co_za/Documents/Documents/Main-Documents/Personal/Blog_Vebash/content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Current-Work\Blog_Vebash\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{ACFAD094-D8EA-4FAF-B074-F0F2496E58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{340CFB8B-72FE-4AAE-92D3-CBFBE05A65A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CB4E48-ED98-4700-A10C-3EE81AF98064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-2200" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>title</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>images/markus-spiske-hGb5WqRrWIg-unsplash.jpg</t>
+  </si>
+  <si>
+    <t>https://sciencificity.github.io/rmd-hide-info/</t>
+  </si>
+  <si>
+    <t>Use code chunk options to hide results and plots</t>
+  </si>
+  <si>
+    <t>R; Suppress Plots and Results in report</t>
+  </si>
+  <si>
+    <t>Hide certain plots and results in rendered Rmd</t>
+  </si>
+  <si>
+    <t>images/arseny-togulev-upnf6XRkWho-unsplash.jpg</t>
   </si>
 </sst>
 </file>
@@ -431,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,13 +576,37 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EFCDE127-97E1-4BE0-94AA-C496E3B749CF}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{40BE7616-A0C8-414F-A387-6E215007A00D}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{921C780A-61CE-4A77-B664-9B2D9B6D7079}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{39D3C094-5A18-4378-AB5A-AA7F9EA9EE63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>